<commit_message>
Added one User Story
</commit_message>
<xml_diff>
--- a/Documentation/OneSport - User Stories.xlsx
+++ b/Documentation/OneSport - User Stories.xlsx
@@ -7,30 +7,30 @@
     <sheet state="visible" name="Analysis" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="Z_1CFDB0F2_6CC7_48BE_A397_EE38F9950C61_.wvu.FilterData">'User Stories'!$G$1:$G$74</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_9D2F7925_2A01_4A70_8BDD_4F61DC14DB4A_.wvu.FilterData">'User Stories'!$C$1:$G$74</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_E7144709_AE2E_477E_9937_3D9EDAB378E2_.wvu.FilterData">'User Stories'!$G$1:$G$1017</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_88E1224D_CD07_4940_8BA0_4A335CE805FA_.wvu.FilterData">'User Stories'!$C$1:$G$74</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_8983776C_E93B_402E_9080_AA77450E1BAF_.wvu.FilterData">'User Stories'!$C$1:$G$74</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_F80EAA41_F933_4B42_9FD3_0D0796C47484_.wvu.FilterData">'User Stories'!$C$1:$G$75</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_E163C9BD_E6CB_47AE_9BFF_D9A085A26EA1_.wvu.FilterData">'User Stories'!$C$1:$G$75</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_23DAAABD_3685_4B86_BD19_716395AE0EC9_.wvu.FilterData">'User Stories'!$G$1:$G$1018</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_B1768477_A502_421D_95DE_D384E5DFA078_.wvu.FilterData">'User Stories'!$G$1:$G$75</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_8F3B4ED6_8AF1_44C1_9AB0_D316D122F059_.wvu.FilterData">'User Stories'!$C$1:$G$75</definedName>
   </definedNames>
   <calcPr/>
   <customWorkbookViews>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{8983776C-E93B-402E-9080-AA77450E1BAF}" name="v2.x"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{9D2F7925-2A01-4A70-8BDD-4F61DC14DB4A}" name="v3.x"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{88E1224D-CD07-4940-8BA0-4A335CE805FA}" name="v1.x"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{E7144709-AE2E-477E-9937-3D9EDAB378E2}" name="Icebox"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{1CFDB0F2-6CC7-48BE-A397-EE38F9950C61}" name="MVP"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{F80EAA41-F933-4B42-9FD3-0D0796C47484}" name="v2.x"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{8F3B4ED6-8AF1-44C1-9AB0-D316D122F059}" name="v3.x"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{E163C9BD-E6CB-47AE-9BFF-D9A085A26EA1}" name="v1.x"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{23DAAABD-3685-4B86-BD19-716395AE0EC9}" name="Icebox"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{B1768477-A502-421D-95DE-D384E5DFA078}" name="MVP"/>
   </customWorkbookViews>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="JcCNtjSQ3Ip68CPWUbbXxtrJ2ckAE7ITJpJ41lgZ6rQ="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="wfIgCEm42TDgvNUHX5vK6deYtLMYzEJdowBw6Lm9bOA="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="48">
   <si>
     <t xml:space="preserve"> EPIC</t>
   </si>
@@ -161,10 +161,13 @@
     <t>Friends</t>
   </si>
   <si>
-    <t>As a User, I want to send a friend request to another user, in order to add him to my friend list</t>
+    <t>As a User, I want to see all my friends</t>
   </si>
   <si>
     <t>4.x</t>
+  </si>
+  <si>
+    <t>As a User, I want to send a friend request to another user, in order to add him to my friend list</t>
   </si>
   <si>
     <t>As a User, I want to check if someone has sent me a friend request, in order to accept or delete it</t>
@@ -1303,16 +1306,16 @@
         <v>45</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D18" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E18" s="16" t="s">
-        <v>17</v>
+      <c r="E18" s="14" t="s">
+        <v>25</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="G18" s="15" t="s">
         <v>44</v>
@@ -1332,10 +1335,10 @@
         <v>25</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F19" s="15" t="s">
         <v>18</v>
@@ -1348,13 +1351,27 @@
       <c r="U19" s="13"/>
     </row>
     <row r="20" ht="22.5" customHeight="1">
-      <c r="A20" s="6"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
+      <c r="A20" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="E20" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="G20" s="15" t="s">
+        <v>44</v>
+      </c>
       <c r="S20" s="11"/>
       <c r="T20" s="12"/>
       <c r="U20" s="13"/>
@@ -1373,7 +1390,7 @@
     </row>
     <row r="22" ht="22.5" customHeight="1">
       <c r="A22" s="6"/>
-      <c r="B22" s="17"/>
+      <c r="B22" s="7"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
@@ -1384,7 +1401,7 @@
       <c r="U22" s="13"/>
     </row>
     <row r="23" ht="22.5" customHeight="1">
-      <c r="A23" s="18"/>
+      <c r="A23" s="6"/>
       <c r="B23" s="17"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
@@ -1587,7 +1604,7 @@
       <c r="T39" s="12"/>
       <c r="U39" s="13"/>
     </row>
-    <row r="40" ht="39.75" customHeight="1">
+    <row r="40" ht="22.5" customHeight="1">
       <c r="A40" s="18"/>
       <c r="B40" s="17"/>
       <c r="C40" s="8"/>
@@ -1599,7 +1616,7 @@
       <c r="T40" s="12"/>
       <c r="U40" s="13"/>
     </row>
-    <row r="41" ht="15.75" customHeight="1">
+    <row r="41" ht="39.75" customHeight="1">
       <c r="A41" s="18"/>
       <c r="B41" s="17"/>
       <c r="C41" s="8"/>
@@ -13455,10 +13472,22 @@
       <c r="T1028" s="12"/>
       <c r="U1028" s="13"/>
     </row>
+    <row r="1029" ht="15.75" customHeight="1">
+      <c r="A1029" s="18"/>
+      <c r="B1029" s="17"/>
+      <c r="C1029" s="8"/>
+      <c r="D1029" s="8"/>
+      <c r="E1029" s="8"/>
+      <c r="F1029" s="10"/>
+      <c r="G1029" s="10"/>
+      <c r="S1029" s="11"/>
+      <c r="T1029" s="12"/>
+      <c r="U1029" s="13"/>
+    </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{1CFDB0F2-6CC7-48BE-A397-EE38F9950C61}" filter="1" showAutoFilter="1">
-      <autoFilter ref="$G$1:$G$74">
+    <customSheetView guid="{B1768477-A502-421D-95DE-D384E5DFA078}" filter="1" showAutoFilter="1">
+      <autoFilter ref="$G$1:$G$75">
         <filterColumn colId="0">
           <customFilters>
             <customFilter val="4.x"/>
@@ -13471,16 +13500,16 @@
         </ext>
       </extLst>
     </customSheetView>
-    <customSheetView guid="{8983776C-E93B-402E-9080-AA77450E1BAF}" filter="1" showAutoFilter="1">
-      <autoFilter ref="$C$1:$G$74"/>
+    <customSheetView guid="{F80EAA41-F933-4B42-9FD3-0D0796C47484}" filter="1" showAutoFilter="1">
+      <autoFilter ref="$C$1:$G$75"/>
       <extLst>
         <ext uri="GoogleSheetsCustomDataVersion1">
           <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" filterViewId="1134550416"/>
         </ext>
       </extLst>
     </customSheetView>
-    <customSheetView guid="{E7144709-AE2E-477E-9937-3D9EDAB378E2}" filter="1" showAutoFilter="1">
-      <autoFilter ref="$G$1:$G$1017">
+    <customSheetView guid="{23DAAABD-3685-4B86-BD19-716395AE0EC9}" filter="1" showAutoFilter="1">
+      <autoFilter ref="$G$1:$G$1018">
         <filterColumn colId="0">
           <customFilters>
             <customFilter val="4.x"/>
@@ -13493,16 +13522,16 @@
         </ext>
       </extLst>
     </customSheetView>
-    <customSheetView guid="{9D2F7925-2A01-4A70-8BDD-4F61DC14DB4A}" filter="1" showAutoFilter="1">
-      <autoFilter ref="$C$1:$G$74"/>
+    <customSheetView guid="{8F3B4ED6-8AF1-44C1-9AB0-D316D122F059}" filter="1" showAutoFilter="1">
+      <autoFilter ref="$C$1:$G$75"/>
       <extLst>
         <ext uri="GoogleSheetsCustomDataVersion1">
           <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" filterViewId="1844978715"/>
         </ext>
       </extLst>
     </customSheetView>
-    <customSheetView guid="{88E1224D-CD07-4940-8BA0-4A335CE805FA}" filter="1" showAutoFilter="1">
-      <autoFilter ref="$C$1:$G$74"/>
+    <customSheetView guid="{E163C9BD-E6CB-47AE-9BFF-D9A085A26EA1}" filter="1" showAutoFilter="1">
+      <autoFilter ref="$C$1:$G$75"/>
       <extLst>
         <ext uri="GoogleSheetsCustomDataVersion1">
           <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" filterViewId="325154005"/>
@@ -13510,189 +13539,189 @@
       </extLst>
     </customSheetView>
   </customSheetViews>
-  <conditionalFormatting sqref="E41:E46">
+  <conditionalFormatting sqref="E42:E47">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="1">
-      <formula>NOT(ISERROR(SEARCH(("1"),(E41))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("1"),(E42))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E41:E46">
+  <conditionalFormatting sqref="E42:E47">
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="2">
-      <formula>NOT(ISERROR(SEARCH(("2"),(E41))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("2"),(E42))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E41:E46">
+  <conditionalFormatting sqref="E42:E47">
     <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="3">
-      <formula>NOT(ISERROR(SEARCH(("3"),(E41))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("3"),(E42))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E41:E46">
+  <conditionalFormatting sqref="E42:E47">
     <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="4">
-      <formula>NOT(ISERROR(SEARCH(("4"),(E41))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("4"),(E42))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F1028">
+  <conditionalFormatting sqref="F2:F1029">
     <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"?"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F1028">
+  <conditionalFormatting sqref="F2:F1029">
     <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F1028">
+  <conditionalFormatting sqref="F2:F1029">
     <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F1028">
+  <conditionalFormatting sqref="F2:F1029">
     <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F1028">
+  <conditionalFormatting sqref="F2:F1029">
     <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F1028">
+  <conditionalFormatting sqref="F2:F1029">
     <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F1028">
+  <conditionalFormatting sqref="F2:F1029">
     <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F1028">
+  <conditionalFormatting sqref="F2:F1029">
     <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F1028">
+  <conditionalFormatting sqref="F2:F1029">
     <cfRule type="cellIs" dxfId="12" priority="13" operator="equal">
       <formula>13</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F1028">
+  <conditionalFormatting sqref="F2:F1029">
     <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
       <formula>21</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F1028">
+  <conditionalFormatting sqref="F2:F1029">
     <cfRule type="cellIs" dxfId="14" priority="15" operator="equal">
       <formula>34</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F1028">
+  <conditionalFormatting sqref="F2:F1029">
     <cfRule type="cellIs" dxfId="15" priority="16" operator="equal">
       <formula>55</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F1028">
+  <conditionalFormatting sqref="F2:F1029">
     <cfRule type="cellIs" dxfId="16" priority="17" operator="equal">
       <formula>89</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F1028">
+  <conditionalFormatting sqref="F2:F1029">
     <cfRule type="cellIs" dxfId="6" priority="18" operator="equal">
       <formula>"XSM"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F1028">
+  <conditionalFormatting sqref="F2:F1029">
     <cfRule type="cellIs" dxfId="8" priority="19" operator="equal">
       <formula>"SM"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F1028">
+  <conditionalFormatting sqref="F2:F1029">
     <cfRule type="cellIs" dxfId="10" priority="20" operator="equal">
       <formula>"MD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F1028">
+  <conditionalFormatting sqref="F2:F1029">
     <cfRule type="cellIs" dxfId="12" priority="21" operator="equal">
       <formula>"LG"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F1028">
+  <conditionalFormatting sqref="F2:F1029">
     <cfRule type="cellIs" dxfId="14" priority="22" operator="equal">
       <formula>"XLG"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F1028">
+  <conditionalFormatting sqref="F2:F1029">
     <cfRule type="cellIs" dxfId="16" priority="23" operator="equal">
       <formula>"XXLG"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C40 C47:C1028">
+  <conditionalFormatting sqref="C1:C41 C48:C1029">
     <cfRule type="containsText" dxfId="17" priority="24" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH(("1"),(C1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C40 C47:C1028">
+  <conditionalFormatting sqref="C1:C41 C48:C1029">
     <cfRule type="containsText" dxfId="18" priority="25" operator="containsText" text="2">
       <formula>NOT(ISERROR(SEARCH(("2"),(C1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C40 C47:C1028">
+  <conditionalFormatting sqref="C1:C41 C48:C1029">
     <cfRule type="containsText" dxfId="19" priority="26" operator="containsText" text="3">
       <formula>NOT(ISERROR(SEARCH(("3"),(C1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C40 C47:C1028">
+  <conditionalFormatting sqref="C1:C41 C48:C1029">
     <cfRule type="containsText" dxfId="20" priority="27" operator="containsText" text="4">
       <formula>NOT(ISERROR(SEARCH(("4"),(C1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1:D1028 C41:C46">
+  <conditionalFormatting sqref="D1:D1029 C42:C47">
     <cfRule type="containsText" dxfId="0" priority="28" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH(("1"),(D1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1:D1028 C41:C46">
+  <conditionalFormatting sqref="D1:D1029 C42:C47">
     <cfRule type="containsText" dxfId="1" priority="29" operator="containsText" text="2">
       <formula>NOT(ISERROR(SEARCH(("2"),(D1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1:D1028 C41:C46">
+  <conditionalFormatting sqref="D1:D1029 C42:C47">
     <cfRule type="containsText" dxfId="2" priority="30" operator="containsText" text="3">
       <formula>NOT(ISERROR(SEARCH(("3"),(D1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1:D1028 C41:C46">
+  <conditionalFormatting sqref="D1:D1029 C42:C47">
     <cfRule type="containsText" dxfId="3" priority="31" operator="containsText" text="4">
       <formula>NOT(ISERROR(SEARCH(("4"),(D1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E40 E45:E1028">
+  <conditionalFormatting sqref="E1:E41 E46:E1029">
     <cfRule type="containsText" dxfId="21" priority="32" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH(("1"),(E1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E40 E45:E1028">
+  <conditionalFormatting sqref="E1:E41 E46:E1029">
     <cfRule type="containsText" dxfId="22" priority="33" operator="containsText" text="2">
       <formula>NOT(ISERROR(SEARCH(("2"),(E1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E40 E45:E1028">
+  <conditionalFormatting sqref="E1:E41 E46:E1029">
     <cfRule type="containsText" dxfId="23" priority="34" operator="containsText" text="3">
       <formula>NOT(ISERROR(SEARCH(("3"),(E1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E40 E45:E1028">
+  <conditionalFormatting sqref="E1:E41 E46:E1029">
     <cfRule type="containsText" dxfId="24" priority="35" operator="containsText" text="4">
       <formula>NOT(ISERROR(SEARCH(("4"),(E1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" sqref="C2:E1028">
+    <dataValidation type="list" allowBlank="1" sqref="C2:E1029">
       <formula1>"1 High,2 Med,3 Med,4 Low"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="F2:F1028">
+    <dataValidation type="list" allowBlank="1" sqref="F2:F1029">
       <formula1>"XSM,SM,MD,LG,XLG,XXLG,0,0.5,1,2,3,5,8,13,21,34,55,89,?"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="G2:G1028">
+    <dataValidation type="list" allowBlank="1" sqref="G2:G1029">
       <formula1>"MVP,1.0,1.x,2.0,2.x,3.0,3.x,4.x"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>